<commit_message>
CIERRE 13 DIC 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #10 OCTUBRE 2023/BALANCE  ZAVALETA   OCTUBRE  2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #10 OCTUBRE 2023/BALANCE  ZAVALETA   OCTUBRE  2023.xlsx
@@ -793,7 +793,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="1231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="1232">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -4486,6 +4486,9 @@
   </si>
   <si>
     <t>Vacaciones Daniela--KAREN</t>
+  </si>
+  <si>
+    <t>ACEITE-VINAGRE-QUESOS-PASTOR-</t>
   </si>
 </sst>
 </file>
@@ -7488,6 +7491,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="11" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="22" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7562,39 +7604,6 @@
     </xf>
     <xf numFmtId="44" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7679,12 +7688,6 @@
     </xf>
     <xf numFmtId="165" fontId="17" fillId="25" borderId="93" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="22" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12397,23 +12400,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -12423,24 +12426,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="640" t="s">
+      <c r="R3" s="653" t="s">
         <v>3</v>
       </c>
     </row>
@@ -12455,14 +12458,14 @@
       <c r="D4" s="24">
         <v>44892</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -12472,11 +12475,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="641"/>
+      <c r="R4" s="654"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -14311,11 +14314,11 @@
       <c r="J49" s="74"/>
       <c r="K49" s="85"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
         <v>1399609.5</v>
       </c>
-      <c r="N49" s="651">
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
         <v>910600</v>
       </c>
@@ -14323,7 +14326,7 @@
         <f>SUM(P5:P40)</f>
         <v>3236981.46</v>
       </c>
-      <c r="Q49" s="663">
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
         <v>-199</v>
       </c>
@@ -14344,10 +14347,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="88"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>571934</v>
@@ -14402,11 +14405,11 @@
       <c r="J53" s="74"/>
       <c r="K53" s="48"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
         <v>2310209.5</v>
       </c>
-      <c r="N53" s="666"/>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -14831,26 +14834,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="659" t="s">
+      <c r="H77" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="660"/>
+      <c r="I77" s="673"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="661">
+      <c r="K77" s="674">
         <f>I75+L75</f>
         <v>1552957.04</v>
       </c>
-      <c r="L77" s="662"/>
+      <c r="L77" s="675"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="653" t="s">
+      <c r="D78" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="653"/>
+      <c r="E78" s="666"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>-123007.98000000021</v>
@@ -14859,22 +14862,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="654" t="s">
+      <c r="D79" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="654"/>
+      <c r="E79" s="667"/>
       <c r="F79" s="101">
         <v>-1513561.68</v>
       </c>
-      <c r="I79" s="655" t="s">
+      <c r="I79" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="656"/>
-      <c r="K79" s="657">
+      <c r="J79" s="669"/>
+      <c r="K79" s="670">
         <f>F81+F82+F83</f>
         <v>1950142.8099999996</v>
       </c>
-      <c r="L79" s="657"/>
+      <c r="L79" s="670"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -14915,11 +14918,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="658">
+      <c r="K81" s="671">
         <f>-C4</f>
         <v>-3445405.07</v>
       </c>
-      <c r="L81" s="657"/>
+      <c r="L81" s="670"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -14936,22 +14939,22 @@
       <c r="C83" s="172">
         <v>44955</v>
       </c>
-      <c r="D83" s="646" t="s">
+      <c r="D83" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="647"/>
+      <c r="E83" s="660"/>
       <c r="F83" s="173">
         <v>3504178.07</v>
       </c>
-      <c r="I83" s="648" t="s">
+      <c r="I83" s="661" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="649"/>
-      <c r="K83" s="650">
+      <c r="J83" s="662"/>
+      <c r="K83" s="663">
         <f>K79+K81</f>
         <v>-1495262.2600000002</v>
       </c>
-      <c r="L83" s="650"/>
+      <c r="L83" s="663"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -15098,12 +15101,6 @@
     <sortCondition ref="J33:J44"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -15120,6 +15117,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -16289,10 +16292,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="679" t="s">
+      <c r="I37" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="680"/>
+      <c r="J37" s="682"/>
       <c r="K37" s="491"/>
       <c r="L37" s="491"/>
       <c r="M37" s="101"/>
@@ -16311,8 +16314,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I38" s="681"/>
-      <c r="J38" s="682"/>
+      <c r="I38" s="683"/>
+      <c r="J38" s="684"/>
       <c r="K38" s="490"/>
       <c r="L38" s="218"/>
       <c r="M38" s="101"/>
@@ -16331,8 +16334,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I39" s="683"/>
-      <c r="J39" s="684"/>
+      <c r="I39" s="685"/>
+      <c r="J39" s="686"/>
       <c r="K39" s="84"/>
       <c r="L39" s="238"/>
       <c r="M39" s="84"/>
@@ -16890,10 +16893,10 @@
         <f>SUM(G3:G66)</f>
         <v>1542483.7999999996</v>
       </c>
-      <c r="I67" s="685" t="s">
+      <c r="I67" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="686"/>
+      <c r="J67" s="688"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>113965</v>
@@ -16915,11 +16918,11 @@
       </c>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="689" t="s">
+      <c r="G68" s="691" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="694"/>
-      <c r="J68" s="695"/>
+      <c r="I68" s="696"/>
+      <c r="J68" s="697"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -16930,7 +16933,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="690"/>
+      <c r="G69" s="692"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -17518,23 +17521,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>642</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -17544,27 +17547,27 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
         <v>509</v>
       </c>
-      <c r="R3" s="696" t="s">
+      <c r="R3" s="698" t="s">
         <v>3</v>
       </c>
     </row>
@@ -17579,14 +17582,14 @@
       <c r="D4" s="24">
         <v>45079</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -17596,11 +17599,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="697"/>
+      <c r="R4" s="699"/>
     </row>
     <row r="5" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="504" t="s">
@@ -19656,11 +19659,11 @@
       <c r="L49" s="49">
         <v>14500</v>
       </c>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
         <v>1601794.8800000001</v>
       </c>
-      <c r="N49" s="651">
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
         <v>1523056</v>
       </c>
@@ -19668,7 +19671,7 @@
         <f>SUM(P5:P40)</f>
         <v>3794729.3800000004</v>
       </c>
-      <c r="Q49" s="663">
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
         <v>-422.61999999999534</v>
       </c>
@@ -19701,10 +19704,10 @@
       <c r="L50" s="89">
         <v>2808.6</v>
       </c>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>1095</v>
@@ -19789,11 +19792,11 @@
       <c r="L53" s="49">
         <v>6254.95</v>
       </c>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
         <v>3124850.88</v>
       </c>
-      <c r="N53" s="666"/>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -20122,26 +20125,26 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="659" t="s">
+      <c r="H69" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="660"/>
+      <c r="I69" s="673"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="661">
+      <c r="K69" s="674">
         <f>I67+L67</f>
         <v>513056.63999999996</v>
       </c>
-      <c r="L69" s="662"/>
+      <c r="L69" s="675"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="653" t="s">
+      <c r="D70" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="653"/>
+      <c r="E70" s="666"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
         <v>1446986.8899999997</v>
@@ -20150,23 +20153,23 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="654" t="s">
+      <c r="D71" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="654"/>
+      <c r="E71" s="667"/>
       <c r="F71" s="101">
         <f>-'   COMPRAS     JUNIO     2023  '!G67</f>
         <v>-1585182.9300000004</v>
       </c>
-      <c r="I71" s="655" t="s">
+      <c r="I71" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="656"/>
-      <c r="K71" s="657">
+      <c r="J71" s="669"/>
+      <c r="K71" s="670">
         <f>F73+F74+F75</f>
         <v>3054589.7999999993</v>
       </c>
-      <c r="L71" s="657"/>
+      <c r="L71" s="670"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160"/>
@@ -20208,11 +20211,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="658">
+      <c r="K73" s="671">
         <f>-C4</f>
         <v>-3897967.53</v>
       </c>
-      <c r="L73" s="657"/>
+      <c r="L73" s="670"/>
     </row>
     <row r="74" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="171" t="s">
@@ -20229,22 +20232,22 @@
       <c r="C75" s="172">
         <v>45107</v>
       </c>
-      <c r="D75" s="646" t="s">
+      <c r="D75" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="647"/>
+      <c r="E75" s="660"/>
       <c r="F75" s="173">
         <v>3131387.04</v>
       </c>
-      <c r="I75" s="648" t="s">
+      <c r="I75" s="661" t="s">
         <v>764</v>
       </c>
-      <c r="J75" s="649"/>
-      <c r="K75" s="650">
+      <c r="J75" s="662"/>
+      <c r="K75" s="663">
         <f>K71+K73</f>
         <v>-843377.73000000045</v>
       </c>
-      <c r="L75" s="650"/>
+      <c r="L75" s="663"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -20392,6 +20395,12 @@
     <sortCondition ref="B37:B49"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -20408,12 +20417,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -21583,10 +21586,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="679" t="s">
+      <c r="I37" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="680"/>
+      <c r="J37" s="682"/>
       <c r="K37" s="491"/>
       <c r="L37" s="491"/>
       <c r="M37" s="101"/>
@@ -21605,8 +21608,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I38" s="681"/>
-      <c r="J38" s="682"/>
+      <c r="I38" s="683"/>
+      <c r="J38" s="684"/>
       <c r="K38" s="490"/>
       <c r="L38" s="218"/>
       <c r="M38" s="101"/>
@@ -21625,8 +21628,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I39" s="683"/>
-      <c r="J39" s="684"/>
+      <c r="I39" s="685"/>
+      <c r="J39" s="686"/>
       <c r="K39" s="84"/>
       <c r="L39" s="238"/>
       <c r="M39" s="84"/>
@@ -22184,10 +22187,10 @@
         <f>SUM(G3:G66)</f>
         <v>1585182.9300000004</v>
       </c>
-      <c r="I67" s="685" t="s">
+      <c r="I67" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="686"/>
+      <c r="J67" s="688"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>121417.2</v>
@@ -22209,11 +22212,11 @@
       </c>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="689" t="s">
+      <c r="G68" s="691" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="694"/>
-      <c r="J68" s="695"/>
+      <c r="I68" s="696"/>
+      <c r="J68" s="697"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -22224,7 +22227,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="690"/>
+      <c r="G69" s="692"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -22813,23 +22816,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>765</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -22839,25 +22842,25 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
-      <c r="R3" s="696" t="s">
+      <c r="R3" s="698" t="s">
         <v>3</v>
       </c>
     </row>
@@ -22872,14 +22875,14 @@
       <c r="D4" s="24">
         <v>45107</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -22889,11 +22892,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="697"/>
+      <c r="R4" s="699"/>
     </row>
     <row r="5" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="504" t="s">
@@ -25022,11 +25025,11 @@
       <c r="L49" s="49">
         <v>5250</v>
       </c>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
         <v>2422108.7600000002</v>
       </c>
-      <c r="N49" s="651">
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
         <v>1603736</v>
       </c>
@@ -25034,7 +25037,7 @@
         <f>SUM(P5:P40)</f>
         <v>4927758.76</v>
       </c>
-      <c r="Q49" s="663">
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
         <v>-0.23999999999068677</v>
       </c>
@@ -25067,10 +25070,10 @@
       <c r="L50" s="89">
         <v>3420</v>
       </c>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>440369</v>
@@ -25161,11 +25164,11 @@
       <c r="L53" s="49">
         <v>8015.92</v>
       </c>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
         <v>4025844.7600000002</v>
       </c>
-      <c r="N53" s="666"/>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -25542,26 +25545,26 @@
       <c r="A69" s="152"/>
       <c r="B69" s="153"/>
       <c r="C69" s="1"/>
-      <c r="H69" s="659" t="s">
+      <c r="H69" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="660"/>
+      <c r="I69" s="673"/>
       <c r="J69" s="154"/>
-      <c r="K69" s="661">
+      <c r="K69" s="674">
         <f>I67+L67</f>
         <v>792651.90999999992</v>
       </c>
-      <c r="L69" s="662"/>
+      <c r="L69" s="675"/>
       <c r="M69" s="155"/>
       <c r="N69" s="155"/>
       <c r="P69" s="44"/>
       <c r="Q69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D70" s="653" t="s">
+      <c r="D70" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="653"/>
+      <c r="E70" s="666"/>
       <c r="F70" s="156">
         <f>F67-K69-C67</f>
         <v>896993.63999999966</v>
@@ -25570,22 +25573,22 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D71" s="654" t="s">
+      <c r="D71" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E71" s="654"/>
+      <c r="E71" s="667"/>
       <c r="F71" s="101">
         <v>-931631.77</v>
       </c>
-      <c r="I71" s="655" t="s">
+      <c r="I71" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J71" s="656"/>
-      <c r="K71" s="657">
+      <c r="J71" s="669"/>
+      <c r="K71" s="670">
         <f>F73+F74+F75</f>
         <v>2818686.5799999996</v>
       </c>
-      <c r="L71" s="657"/>
+      <c r="L71" s="670"/>
       <c r="M71" s="159"/>
       <c r="N71" s="159"/>
       <c r="O71" s="160">
@@ -25630,11 +25633,11 @@
         <v>21</v>
       </c>
       <c r="J73" s="170"/>
-      <c r="K73" s="658">
+      <c r="K73" s="671">
         <f>-C4</f>
         <v>-3131387.04</v>
       </c>
-      <c r="L73" s="657"/>
+      <c r="L73" s="670"/>
       <c r="O73" s="536">
         <f>SUM(O71:O72)</f>
         <v>104</v>
@@ -25655,22 +25658,22 @@
       <c r="C75" s="172">
         <v>45135</v>
       </c>
-      <c r="D75" s="646" t="s">
+      <c r="D75" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="647"/>
+      <c r="E75" s="660"/>
       <c r="F75" s="173">
         <v>2820551.31</v>
       </c>
-      <c r="I75" s="648" t="s">
+      <c r="I75" s="661" t="s">
         <v>220</v>
       </c>
-      <c r="J75" s="649"/>
-      <c r="K75" s="650">
+      <c r="J75" s="662"/>
+      <c r="K75" s="663">
         <f>K71+K73</f>
         <v>-312700.46000000043</v>
       </c>
-      <c r="L75" s="650"/>
+      <c r="L75" s="663"/>
     </row>
     <row r="76" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C76" s="174"/>
@@ -25818,6 +25821,12 @@
     <sortCondition ref="J40:J62"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -25834,12 +25843,6 @@
     <mergeCell ref="H69:I69"/>
     <mergeCell ref="K69:L69"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -27107,10 +27110,10 @@
         <f t="shared" si="0"/>
         <v>9903.85</v>
       </c>
-      <c r="I37" s="679" t="s">
+      <c r="I37" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="680"/>
+      <c r="J37" s="682"/>
       <c r="K37" s="491"/>
       <c r="L37" s="491"/>
       <c r="M37" s="101"/>
@@ -27135,8 +27138,8 @@
         <f t="shared" si="0"/>
         <v>11767.68</v>
       </c>
-      <c r="I38" s="681"/>
-      <c r="J38" s="682"/>
+      <c r="I38" s="683"/>
+      <c r="J38" s="684"/>
       <c r="K38" s="490"/>
       <c r="L38" s="218"/>
       <c r="M38" s="101"/>
@@ -27161,8 +27164,8 @@
         <f t="shared" si="0"/>
         <v>24157.14</v>
       </c>
-      <c r="I39" s="683"/>
-      <c r="J39" s="684"/>
+      <c r="I39" s="685"/>
+      <c r="J39" s="686"/>
       <c r="K39" s="84"/>
       <c r="L39" s="238"/>
       <c r="M39" s="84"/>
@@ -27768,10 +27771,10 @@
         <f>SUM(G3:G66)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I67" s="685" t="s">
+      <c r="I67" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="686"/>
+      <c r="J67" s="688"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>122543.6</v>
@@ -27793,11 +27796,11 @@
       </c>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="689" t="s">
+      <c r="G68" s="691" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="694"/>
-      <c r="J68" s="695"/>
+      <c r="I68" s="696"/>
+      <c r="J68" s="697"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -27808,7 +27811,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="690"/>
+      <c r="G69" s="692"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -28396,23 +28399,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>765</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -28422,25 +28425,25 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
-      <c r="R3" s="696" t="s">
+      <c r="R3" s="698" t="s">
         <v>3</v>
       </c>
     </row>
@@ -28455,14 +28458,14 @@
       <c r="D4" s="24">
         <v>45135</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -28472,11 +28475,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="697"/>
+      <c r="R4" s="699"/>
     </row>
     <row r="5" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="504" t="s">
@@ -30703,11 +30706,11 @@
       <c r="J49" s="338"/>
       <c r="K49" s="349"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
         <v>2901103.23</v>
       </c>
-      <c r="N49" s="651">
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
         <v>2054394</v>
       </c>
@@ -30715,7 +30718,7 @@
         <f>SUM(P5:P40)</f>
         <v>6121324.54</v>
       </c>
-      <c r="Q49" s="663">
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
         <v>-1197.4599999999919</v>
       </c>
@@ -30748,10 +30751,10 @@
       <c r="L50" s="89">
         <v>2958</v>
       </c>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>146522</v>
@@ -30842,11 +30845,11 @@
       <c r="L53" s="49">
         <v>1100.01</v>
       </c>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
         <v>4955497.2300000004</v>
       </c>
-      <c r="N53" s="666"/>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -31561,26 +31564,26 @@
       <c r="A81" s="152"/>
       <c r="B81" s="153"/>
       <c r="C81" s="1"/>
-      <c r="H81" s="659" t="s">
+      <c r="H81" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I81" s="660"/>
+      <c r="I81" s="673"/>
       <c r="J81" s="154"/>
-      <c r="K81" s="661">
+      <c r="K81" s="674">
         <f>I79+L79</f>
         <v>778945.87000000011</v>
       </c>
-      <c r="L81" s="662"/>
+      <c r="L81" s="675"/>
       <c r="M81" s="155"/>
       <c r="N81" s="155"/>
       <c r="P81" s="44"/>
       <c r="Q81" s="19"/>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D82" s="653" t="s">
+      <c r="D82" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E82" s="653"/>
+      <c r="E82" s="666"/>
       <c r="F82" s="156">
         <f>F79-K81-C79</f>
         <v>1583916.4599999995</v>
@@ -31589,22 +31592,22 @@
       <c r="J82" s="158"/>
     </row>
     <row r="83" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D83" s="654" t="s">
+      <c r="D83" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E83" s="654"/>
+      <c r="E83" s="667"/>
       <c r="F83" s="101">
         <v>-1249902.31</v>
       </c>
-      <c r="I83" s="655" t="s">
+      <c r="I83" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J83" s="656"/>
-      <c r="K83" s="657">
+      <c r="J83" s="669"/>
+      <c r="K83" s="670">
         <f>F85+F86+F87</f>
         <v>3373322.2099999995</v>
       </c>
-      <c r="L83" s="657"/>
+      <c r="L83" s="670"/>
       <c r="M83" s="159"/>
       <c r="N83" s="159"/>
       <c r="O83" s="160"/>
@@ -31645,11 +31648,11 @@
         <v>21</v>
       </c>
       <c r="J85" s="170"/>
-      <c r="K85" s="658">
+      <c r="K85" s="671">
         <f>-C4</f>
         <v>-2820551.31</v>
       </c>
-      <c r="L85" s="657"/>
+      <c r="L85" s="670"/>
       <c r="O85" s="536"/>
     </row>
     <row r="86" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -31667,22 +31670,22 @@
       <c r="C87" s="172">
         <v>45171</v>
       </c>
-      <c r="D87" s="646" t="s">
+      <c r="D87" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E87" s="647"/>
+      <c r="E87" s="660"/>
       <c r="F87" s="173">
         <v>3146460.66</v>
       </c>
-      <c r="I87" s="698" t="s">
+      <c r="I87" s="700" t="s">
         <v>1143</v>
       </c>
-      <c r="J87" s="699"/>
-      <c r="K87" s="700">
+      <c r="J87" s="701"/>
+      <c r="K87" s="702">
         <f>K83+K85</f>
         <v>552770.89999999944</v>
       </c>
-      <c r="L87" s="700"/>
+      <c r="L87" s="702"/>
     </row>
     <row r="88" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C88" s="174"/>
@@ -31830,12 +31833,6 @@
     <sortCondition ref="B44:B74"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -31852,6 +31849,12 @@
     <mergeCell ref="H81:I81"/>
     <mergeCell ref="K81:L81"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -33593,10 +33596,10 @@
         <f t="shared" si="0"/>
         <v>11880</v>
       </c>
-      <c r="I49" s="679" t="s">
+      <c r="I49" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J49" s="680"/>
+      <c r="J49" s="682"/>
       <c r="K49" s="108"/>
       <c r="L49" s="177"/>
       <c r="M49" s="44"/>
@@ -33621,8 +33624,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I50" s="681"/>
-      <c r="J50" s="682"/>
+      <c r="I50" s="683"/>
+      <c r="J50" s="684"/>
       <c r="K50" s="108"/>
       <c r="L50" s="177"/>
       <c r="M50" s="44"/>
@@ -33647,8 +33650,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I51" s="683"/>
-      <c r="J51" s="684"/>
+      <c r="I51" s="685"/>
+      <c r="J51" s="686"/>
       <c r="K51" s="108"/>
       <c r="L51" s="177"/>
       <c r="M51" s="44"/>
@@ -34008,10 +34011,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I65" s="685" t="s">
+      <c r="I65" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J65" s="686"/>
+      <c r="J65" s="688"/>
       <c r="K65" s="560">
         <f>SUM(K3:K64)</f>
         <v>226585.60000000003</v>
@@ -34040,8 +34043,8 @@
         <f t="shared" ref="G66:G68" si="2">D66-F66</f>
         <v>0</v>
       </c>
-      <c r="I66" s="694"/>
-      <c r="J66" s="695"/>
+      <c r="I66" s="696"/>
+      <c r="J66" s="697"/>
       <c r="K66" s="150"/>
       <c r="L66" s="269"/>
       <c r="M66" s="5"/>
@@ -34117,7 +34120,7 @@
       <c r="D70" s="480"/>
       <c r="E70" s="269"/>
       <c r="F70" s="5"/>
-      <c r="G70" s="689" t="s">
+      <c r="G70" s="691" t="s">
         <v>36</v>
       </c>
       <c r="H70" s="233"/>
@@ -34133,7 +34136,7 @@
       <c r="D71" s="1"/>
       <c r="E71" s="269"/>
       <c r="F71" s="5"/>
-      <c r="G71" s="690"/>
+      <c r="G71" s="692"/>
       <c r="H71" s="233"/>
       <c r="I71" s="303"/>
       <c r="J71" s="550"/>
@@ -34678,54 +34681,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>1082</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="701" t="s">
+      <c r="J2" s="703" t="s">
         <v>1122</v>
       </c>
-      <c r="K2" s="702"/>
-      <c r="L2" s="702"/>
-      <c r="M2" s="703"/>
+      <c r="K2" s="704"/>
+      <c r="L2" s="704"/>
+      <c r="M2" s="705"/>
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
-      <c r="R3" s="696" t="s">
+      <c r="R3" s="698" t="s">
         <v>3</v>
       </c>
     </row>
@@ -34740,14 +34743,14 @@
       <c r="D4" s="24">
         <v>45171</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -34757,11 +34760,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="697"/>
+      <c r="R4" s="699"/>
     </row>
     <row r="5" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="504" t="s">
@@ -36878,11 +36881,11 @@
       <c r="L49" s="369">
         <v>8488</v>
       </c>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
         <v>2549017.7400000002</v>
       </c>
-      <c r="N49" s="651">
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
         <v>1551885</v>
       </c>
@@ -36890,7 +36893,7 @@
         <f>SUM(P5:P40)</f>
         <v>4761795.24</v>
       </c>
-      <c r="Q49" s="663">
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
         <v>5.2399999999906868</v>
       </c>
@@ -36923,10 +36926,10 @@
       <c r="L50" s="369">
         <v>1856</v>
       </c>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>37814</v>
@@ -37011,11 +37014,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
         <v>4100902.74</v>
       </c>
-      <c r="N53" s="666"/>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -37524,26 +37527,26 @@
       <c r="A81" s="152"/>
       <c r="B81" s="153"/>
       <c r="C81" s="1"/>
-      <c r="H81" s="659" t="s">
+      <c r="H81" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I81" s="660"/>
+      <c r="I81" s="673"/>
       <c r="J81" s="154"/>
-      <c r="K81" s="661">
+      <c r="K81" s="674">
         <f>I79+L79</f>
         <v>366832.13999999996</v>
       </c>
-      <c r="L81" s="662"/>
+      <c r="L81" s="675"/>
       <c r="M81" s="155"/>
       <c r="N81" s="155"/>
       <c r="P81" s="44"/>
       <c r="Q81" s="19"/>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D82" s="653" t="s">
+      <c r="D82" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E82" s="653"/>
+      <c r="E82" s="666"/>
       <c r="F82" s="156">
         <f>F79-K81-C79</f>
         <v>1964745.67</v>
@@ -37552,22 +37555,22 @@
       <c r="J82" s="158"/>
     </row>
     <row r="83" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D83" s="654" t="s">
+      <c r="D83" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E83" s="654"/>
+      <c r="E83" s="667"/>
       <c r="F83" s="101">
         <v>0</v>
       </c>
-      <c r="I83" s="655" t="s">
+      <c r="I83" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J83" s="656"/>
-      <c r="K83" s="657">
+      <c r="J83" s="669"/>
+      <c r="K83" s="670">
         <f>F85+F86+F87</f>
         <v>5604393.8799999999</v>
       </c>
-      <c r="L83" s="657"/>
+      <c r="L83" s="670"/>
       <c r="M83" s="159"/>
       <c r="N83" s="159"/>
       <c r="O83" s="160"/>
@@ -37608,11 +37611,11 @@
         <v>21</v>
       </c>
       <c r="J85" s="170"/>
-      <c r="K85" s="658">
+      <c r="K85" s="671">
         <f>-C4</f>
         <v>-3146460.66</v>
       </c>
-      <c r="L85" s="657"/>
+      <c r="L85" s="670"/>
       <c r="O85" s="536"/>
     </row>
     <row r="86" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -37630,20 +37633,20 @@
       <c r="C87" s="172">
         <v>45198</v>
       </c>
-      <c r="D87" s="646" t="s">
+      <c r="D87" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E87" s="647"/>
+      <c r="E87" s="660"/>
       <c r="F87" s="173">
         <v>3340512.21</v>
       </c>
-      <c r="I87" s="648"/>
-      <c r="J87" s="649"/>
-      <c r="K87" s="650">
+      <c r="I87" s="661"/>
+      <c r="J87" s="662"/>
+      <c r="K87" s="663">
         <f>K83+K85</f>
         <v>2457933.2199999997</v>
       </c>
-      <c r="L87" s="650"/>
+      <c r="L87" s="663"/>
     </row>
     <row r="88" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C88" s="174"/>
@@ -37788,13 +37791,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J2:M2"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -37811,6 +37807,13 @@
     <mergeCell ref="H81:I81"/>
     <mergeCell ref="K81:L81"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -39122,10 +39125,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I49" s="679" t="s">
+      <c r="I49" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J49" s="680"/>
+      <c r="J49" s="682"/>
       <c r="K49" s="108"/>
       <c r="L49" s="177"/>
       <c r="M49" s="44"/>
@@ -39144,8 +39147,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I50" s="681"/>
-      <c r="J50" s="682"/>
+      <c r="I50" s="683"/>
+      <c r="J50" s="684"/>
       <c r="K50" s="108"/>
       <c r="L50" s="177"/>
       <c r="M50" s="44"/>
@@ -39164,8 +39167,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I51" s="683"/>
-      <c r="J51" s="684"/>
+      <c r="I51" s="685"/>
+      <c r="J51" s="686"/>
       <c r="K51" s="108"/>
       <c r="L51" s="177"/>
       <c r="M51" s="44"/>
@@ -39441,10 +39444,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I65" s="685" t="s">
+      <c r="I65" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J65" s="686"/>
+      <c r="J65" s="688"/>
       <c r="K65" s="560">
         <f>SUM(K3:K64)</f>
         <v>0</v>
@@ -39467,8 +39470,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I66" s="694"/>
-      <c r="J66" s="695"/>
+      <c r="I66" s="696"/>
+      <c r="J66" s="697"/>
       <c r="K66" s="150"/>
       <c r="L66" s="269"/>
       <c r="M66" s="5"/>
@@ -39532,7 +39535,7 @@
       <c r="D70" s="480"/>
       <c r="E70" s="269"/>
       <c r="F70" s="5"/>
-      <c r="G70" s="689" t="s">
+      <c r="G70" s="691" t="s">
         <v>36</v>
       </c>
       <c r="H70" s="233"/>
@@ -39548,7 +39551,7 @@
       <c r="D71" s="1"/>
       <c r="E71" s="269"/>
       <c r="F71" s="5"/>
-      <c r="G71" s="690"/>
+      <c r="G71" s="692"/>
       <c r="H71" s="233"/>
       <c r="I71" s="303"/>
       <c r="J71" s="550"/>
@@ -40068,7 +40071,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="R17" sqref="R17"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -40094,54 +40097,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>1142</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="701" t="s">
+      <c r="J2" s="703" t="s">
         <v>1122</v>
       </c>
-      <c r="K2" s="702"/>
-      <c r="L2" s="702"/>
-      <c r="M2" s="703"/>
+      <c r="K2" s="704"/>
+      <c r="L2" s="704"/>
+      <c r="M2" s="705"/>
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:22" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="533"/>
-      <c r="R3" s="696" t="s">
+      <c r="R3" s="698" t="s">
         <v>3</v>
       </c>
     </row>
@@ -40156,14 +40159,14 @@
       <c r="D4" s="24">
         <v>45198</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -40173,11 +40176,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="697"/>
+      <c r="R4" s="699"/>
     </row>
     <row r="5" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="504" t="s">
@@ -40273,7 +40276,7 @@
         <v>117181.5</v>
       </c>
       <c r="Q6" s="45">
-        <f t="shared" ref="Q6:Q11" si="1">P6-F6</f>
+        <f t="shared" ref="Q6:Q8" si="1">P6-F6</f>
         <v>4.5</v>
       </c>
       <c r="R6" s="390">
@@ -40531,7 +40534,7 @@
       <c r="J11" s="52">
         <v>45205</v>
       </c>
-      <c r="K11" s="704" t="s">
+      <c r="K11" s="640" t="s">
         <v>1222</v>
       </c>
       <c r="L11" s="49">
@@ -40588,7 +40591,7 @@
       <c r="J12" s="40">
         <v>45206</v>
       </c>
-      <c r="K12" s="705" t="s">
+      <c r="K12" s="641" t="s">
         <v>1224</v>
       </c>
       <c r="L12" s="49">
@@ -40896,33 +40899,42 @@
       <c r="B18" s="32">
         <v>45212</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="621"/>
+      <c r="C18" s="33">
+        <v>11696</v>
+      </c>
+      <c r="D18" s="621" t="s">
+        <v>1231</v>
+      </c>
       <c r="E18" s="35">
         <v>45212</v>
       </c>
-      <c r="F18" s="36"/>
+      <c r="F18" s="36">
+        <v>166672</v>
+      </c>
       <c r="G18" s="37"/>
       <c r="H18" s="38">
         <v>45212</v>
       </c>
-      <c r="I18" s="39"/>
+      <c r="I18" s="39">
+        <v>2471</v>
+      </c>
       <c r="J18" s="40"/>
       <c r="K18" s="616"/>
       <c r="L18" s="49"/>
       <c r="M18" s="42">
-        <v>0</v>
+        <f>85080+5633+539</f>
+        <v>91252</v>
       </c>
       <c r="N18" s="43">
-        <v>0</v>
+        <v>58232</v>
       </c>
       <c r="P18" s="49">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="45">
+        <v>163651</v>
+      </c>
+      <c r="Q18" s="285">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-3021</v>
       </c>
       <c r="R18" s="46" t="s">
         <v>10</v>
@@ -42010,21 +42022,21 @@
       <c r="J49" s="338"/>
       <c r="K49" s="471"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
-        <v>981881.86</v>
-      </c>
-      <c r="N49" s="651">
+        <v>1073133.8599999999</v>
+      </c>
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
-        <v>735488</v>
+        <v>793720</v>
       </c>
       <c r="P49" s="111">
         <f>SUM(P5:P40)</f>
-        <v>2088342.86</v>
-      </c>
-      <c r="Q49" s="663">
+        <v>2251993.8600000003</v>
+      </c>
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
-        <v>4.5</v>
+        <v>-3016.5</v>
       </c>
       <c r="R49" s="46">
         <v>0</v>
@@ -42043,10 +42055,10 @@
       <c r="J50" s="338"/>
       <c r="K50" s="343"/>
       <c r="L50" s="49"/>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>54838</v>
@@ -42101,11 +42113,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
-        <v>1717369.8599999999</v>
-      </c>
-      <c r="N53" s="666"/>
+        <v>1866853.8599999999</v>
+      </c>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -42566,7 +42578,7 @@
       </c>
       <c r="C79" s="519">
         <f>SUM(C5:C78)</f>
-        <v>248110</v>
+        <v>259806</v>
       </c>
       <c r="D79" s="520"/>
       <c r="E79" s="521" t="s">
@@ -42574,7 +42586,7 @@
       </c>
       <c r="F79" s="522">
         <f>SUM(F5:F61)</f>
-        <v>2034751</v>
+        <v>2201423</v>
       </c>
       <c r="G79" s="523"/>
       <c r="H79" s="521" t="s">
@@ -42582,7 +42594,7 @@
       </c>
       <c r="I79" s="524">
         <f>SUM(I5:I61)</f>
-        <v>38884</v>
+        <v>41355</v>
       </c>
       <c r="J79" s="525"/>
       <c r="K79" s="526" t="s">
@@ -42608,50 +42620,50 @@
       <c r="A81" s="152"/>
       <c r="B81" s="153"/>
       <c r="C81" s="1"/>
-      <c r="H81" s="659" t="s">
+      <c r="H81" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I81" s="660"/>
+      <c r="I81" s="673"/>
       <c r="J81" s="154"/>
-      <c r="K81" s="661">
+      <c r="K81" s="674">
         <f>I79+L79</f>
-        <v>174962</v>
-      </c>
-      <c r="L81" s="662"/>
+        <v>177433</v>
+      </c>
+      <c r="L81" s="675"/>
       <c r="M81" s="155"/>
       <c r="N81" s="155"/>
       <c r="P81" s="44"/>
       <c r="Q81" s="19"/>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D82" s="653" t="s">
+      <c r="D82" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E82" s="653"/>
+      <c r="E82" s="666"/>
       <c r="F82" s="156">
         <f>F79-K81-C79</f>
-        <v>1611679</v>
+        <v>1764184</v>
       </c>
       <c r="I82" s="157"/>
       <c r="J82" s="158"/>
     </row>
     <row r="83" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D83" s="654" t="s">
+      <c r="D83" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E83" s="654"/>
+      <c r="E83" s="667"/>
       <c r="F83" s="101">
         <v>0</v>
       </c>
-      <c r="I83" s="655" t="s">
+      <c r="I83" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J83" s="656"/>
-      <c r="K83" s="657">
+      <c r="J83" s="669"/>
+      <c r="K83" s="670">
         <f>F85+F86+F87</f>
-        <v>5385182.4000000004</v>
-      </c>
-      <c r="L83" s="657"/>
+        <v>5537687.4000000004</v>
+      </c>
+      <c r="L83" s="670"/>
       <c r="M83" s="159"/>
       <c r="N83" s="159"/>
       <c r="O83" s="160"/>
@@ -42685,18 +42697,18 @@
       </c>
       <c r="F85" s="150">
         <f>SUM(F82:F84)</f>
-        <v>1611679</v>
+        <v>1764184</v>
       </c>
       <c r="H85" s="168"/>
       <c r="I85" s="169" t="s">
         <v>21</v>
       </c>
       <c r="J85" s="170"/>
-      <c r="K85" s="658">
+      <c r="K85" s="671">
         <f>-C4</f>
         <v>-3340512.21</v>
       </c>
-      <c r="L85" s="657"/>
+      <c r="L85" s="670"/>
       <c r="O85" s="536"/>
     </row>
     <row r="86" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -42714,20 +42726,20 @@
       <c r="C87" s="172">
         <v>45226</v>
       </c>
-      <c r="D87" s="646" t="s">
+      <c r="D87" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E87" s="647"/>
+      <c r="E87" s="660"/>
       <c r="F87" s="173">
         <v>3773503.4</v>
       </c>
-      <c r="I87" s="648"/>
-      <c r="J87" s="649"/>
-      <c r="K87" s="650">
+      <c r="I87" s="661"/>
+      <c r="J87" s="662"/>
+      <c r="K87" s="663">
         <f>K83+K85</f>
-        <v>2044670.1900000004</v>
-      </c>
-      <c r="L87" s="650"/>
+        <v>2197175.1900000004</v>
+      </c>
+      <c r="L87" s="663"/>
     </row>
     <row r="88" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C88" s="174"/>
@@ -42872,6 +42884,18 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="N49:N50"/>
+    <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="P3:P4"/>
     <mergeCell ref="K85:L85"/>
     <mergeCell ref="D87:E87"/>
     <mergeCell ref="I87:J87"/>
@@ -42883,18 +42907,6 @@
     <mergeCell ref="D83:E83"/>
     <mergeCell ref="I83:J83"/>
     <mergeCell ref="K83:L83"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="N49:N50"/>
-    <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -44271,10 +44283,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="676"/>
-      <c r="J36" s="677"/>
-      <c r="K36" s="677"/>
-      <c r="L36" s="678"/>
+      <c r="I36" s="678"/>
+      <c r="J36" s="679"/>
+      <c r="K36" s="679"/>
+      <c r="L36" s="680"/>
       <c r="M36" s="101"/>
       <c r="N36" s="227">
         <f t="shared" si="1"/>
@@ -44301,10 +44313,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="676"/>
-      <c r="J37" s="677"/>
-      <c r="K37" s="677"/>
-      <c r="L37" s="678"/>
+      <c r="I37" s="678"/>
+      <c r="J37" s="679"/>
+      <c r="K37" s="679"/>
+      <c r="L37" s="680"/>
       <c r="M37" s="101"/>
       <c r="N37" s="227">
         <f t="shared" si="1"/>
@@ -44361,10 +44373,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I40" s="679" t="s">
+      <c r="I40" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="680"/>
+      <c r="J40" s="682"/>
       <c r="K40" s="84"/>
       <c r="L40" s="238"/>
       <c r="M40" s="84"/>
@@ -44383,8 +44395,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I41" s="681"/>
-      <c r="J41" s="682"/>
+      <c r="I41" s="683"/>
+      <c r="J41" s="684"/>
       <c r="K41" s="84"/>
       <c r="L41" s="238"/>
       <c r="M41" s="84"/>
@@ -44403,8 +44415,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="683"/>
-      <c r="J42" s="684"/>
+      <c r="I42" s="685"/>
+      <c r="J42" s="686"/>
       <c r="K42" s="84"/>
       <c r="L42" s="238"/>
       <c r="M42" s="84"/>
@@ -44908,10 +44920,10 @@
         <f>SUM(G3:G66)</f>
         <v>0</v>
       </c>
-      <c r="I67" s="685" t="s">
+      <c r="I67" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="686"/>
+      <c r="J67" s="688"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>92013.200000000012</v>
@@ -44931,11 +44943,11 @@
       <c r="D68" s="268"/>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="689" t="s">
+      <c r="G68" s="691" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="687"/>
-      <c r="J68" s="688"/>
+      <c r="I68" s="689"/>
+      <c r="J68" s="690"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -44946,7 +44958,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="690"/>
+      <c r="G69" s="692"/>
       <c r="K69" s="1"/>
       <c r="L69" s="269"/>
       <c r="M69" s="5"/>
@@ -46575,10 +46587,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I49" s="679" t="s">
+      <c r="I49" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J49" s="680"/>
+      <c r="J49" s="682"/>
       <c r="K49" s="108"/>
       <c r="L49" s="177"/>
       <c r="M49" s="44"/>
@@ -46597,8 +46609,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I50" s="681"/>
-      <c r="J50" s="682"/>
+      <c r="I50" s="683"/>
+      <c r="J50" s="684"/>
       <c r="K50" s="108"/>
       <c r="L50" s="177"/>
       <c r="M50" s="44"/>
@@ -46617,8 +46629,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I51" s="683"/>
-      <c r="J51" s="684"/>
+      <c r="I51" s="685"/>
+      <c r="J51" s="686"/>
       <c r="K51" s="108"/>
       <c r="L51" s="177"/>
       <c r="M51" s="44"/>
@@ -46894,10 +46906,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I65" s="685" t="s">
+      <c r="I65" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J65" s="686"/>
+      <c r="J65" s="688"/>
       <c r="K65" s="560">
         <f>SUM(K3:K64)</f>
         <v>0</v>
@@ -46920,8 +46932,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I66" s="694"/>
-      <c r="J66" s="695"/>
+      <c r="I66" s="696"/>
+      <c r="J66" s="697"/>
       <c r="K66" s="150"/>
       <c r="L66" s="269"/>
       <c r="M66" s="5"/>
@@ -46985,7 +46997,7 @@
       <c r="D70" s="480"/>
       <c r="E70" s="269"/>
       <c r="F70" s="5"/>
-      <c r="G70" s="689" t="s">
+      <c r="G70" s="691" t="s">
         <v>36</v>
       </c>
       <c r="H70" s="233"/>
@@ -47001,7 +47013,7 @@
       <c r="D71" s="1"/>
       <c r="E71" s="269"/>
       <c r="F71" s="5"/>
-      <c r="G71" s="690"/>
+      <c r="G71" s="692"/>
       <c r="H71" s="233"/>
       <c r="I71" s="303"/>
       <c r="J71" s="550"/>
@@ -47570,23 +47582,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -47596,24 +47608,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="640" t="s">
+      <c r="R3" s="653" t="s">
         <v>3</v>
       </c>
     </row>
@@ -47628,14 +47640,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -47645,11 +47657,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="641"/>
+      <c r="R4" s="654"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -49625,11 +49637,11 @@
       <c r="L49" s="49">
         <v>5160.4799999999996</v>
       </c>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
         <v>1964337.8699999999</v>
       </c>
-      <c r="N49" s="651">
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
         <v>1314937</v>
       </c>
@@ -49637,7 +49649,7 @@
         <f>SUM(P5:P40)</f>
         <v>3956557.8699999996</v>
       </c>
-      <c r="Q49" s="663">
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
         <v>-996.13000000000466</v>
       </c>
@@ -49670,10 +49682,10 @@
       <c r="L50" s="89">
         <v>4412</v>
       </c>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>16567</v>
@@ -49764,11 +49776,11 @@
       <c r="L53" s="49">
         <v>4698</v>
       </c>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
         <v>3279274.87</v>
       </c>
-      <c r="N53" s="666"/>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -50327,26 +50339,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="659" t="s">
+      <c r="H77" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="660"/>
+      <c r="I77" s="673"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="661">
+      <c r="K77" s="674">
         <f>I75+L75</f>
         <v>526980.64000000013</v>
       </c>
-      <c r="L77" s="662"/>
+      <c r="L77" s="675"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="653" t="s">
+      <c r="D78" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="653"/>
+      <c r="E78" s="666"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1939381.5999999999</v>
@@ -50355,22 +50367,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="654" t="s">
+      <c r="D79" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="654"/>
+      <c r="E79" s="667"/>
       <c r="F79" s="101">
         <v>-1830849.67</v>
       </c>
-      <c r="I79" s="655" t="s">
+      <c r="I79" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="656"/>
-      <c r="K79" s="657">
+      <c r="J79" s="669"/>
+      <c r="K79" s="670">
         <f>F81+F82+F83</f>
         <v>3946521.55</v>
       </c>
-      <c r="L79" s="657"/>
+      <c r="L79" s="670"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -50411,11 +50423,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="658">
+      <c r="K81" s="671">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="657"/>
+      <c r="L81" s="670"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -50432,22 +50444,22 @@
       <c r="C83" s="172">
         <v>44988</v>
       </c>
-      <c r="D83" s="646" t="s">
+      <c r="D83" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="647"/>
+      <c r="E83" s="660"/>
       <c r="F83" s="173">
         <v>3720574.62</v>
       </c>
-      <c r="I83" s="691" t="s">
+      <c r="I83" s="693" t="s">
         <v>25</v>
       </c>
-      <c r="J83" s="692"/>
-      <c r="K83" s="693">
+      <c r="J83" s="694"/>
+      <c r="K83" s="695">
         <f>K79+K81</f>
         <v>442343.48</v>
       </c>
-      <c r="L83" s="693"/>
+      <c r="L83" s="695"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -50594,6 +50606,12 @@
     <sortCondition ref="J46:J65"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -50610,12 +50628,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -52027,10 +52039,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="676"/>
-      <c r="J36" s="677"/>
-      <c r="K36" s="677"/>
-      <c r="L36" s="678"/>
+      <c r="I36" s="678"/>
+      <c r="J36" s="679"/>
+      <c r="K36" s="679"/>
+      <c r="L36" s="680"/>
       <c r="M36" s="101"/>
       <c r="N36" s="227">
         <f t="shared" si="1"/>
@@ -52057,10 +52069,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="676"/>
-      <c r="J37" s="677"/>
-      <c r="K37" s="677"/>
-      <c r="L37" s="678"/>
+      <c r="I37" s="678"/>
+      <c r="J37" s="679"/>
+      <c r="K37" s="679"/>
+      <c r="L37" s="680"/>
       <c r="M37" s="101"/>
       <c r="N37" s="227">
         <f t="shared" si="1"/>
@@ -52127,10 +52139,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I40" s="679" t="s">
+      <c r="I40" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="680"/>
+      <c r="J40" s="682"/>
       <c r="K40" s="84"/>
       <c r="L40" s="238"/>
       <c r="M40" s="84"/>
@@ -52149,8 +52161,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I41" s="681"/>
-      <c r="J41" s="682"/>
+      <c r="I41" s="683"/>
+      <c r="J41" s="684"/>
       <c r="K41" s="84"/>
       <c r="L41" s="238"/>
       <c r="M41" s="84"/>
@@ -52169,8 +52181,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="683"/>
-      <c r="J42" s="684"/>
+      <c r="I42" s="685"/>
+      <c r="J42" s="686"/>
       <c r="K42" s="84"/>
       <c r="L42" s="238"/>
       <c r="M42" s="84"/>
@@ -52674,10 +52686,10 @@
         <f>SUM(G3:G66)</f>
         <v>0</v>
       </c>
-      <c r="I67" s="685" t="s">
+      <c r="I67" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="686"/>
+      <c r="J67" s="688"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>111122</v>
@@ -52697,11 +52709,11 @@
       <c r="D68" s="268"/>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="689" t="s">
+      <c r="G68" s="691" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="694"/>
-      <c r="J68" s="695"/>
+      <c r="I68" s="696"/>
+      <c r="J68" s="697"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -52712,7 +52724,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="690"/>
+      <c r="G69" s="692"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -53327,23 +53339,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>238</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -53353,24 +53365,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="696" t="s">
+      <c r="R3" s="698" t="s">
         <v>3</v>
       </c>
     </row>
@@ -53385,14 +53397,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -53402,11 +53414,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="697"/>
+      <c r="R4" s="699"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -55387,11 +55399,11 @@
       <c r="L49" s="376">
         <v>6074.64</v>
       </c>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
         <v>1803019.98</v>
       </c>
-      <c r="N49" s="651">
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
         <v>1138524</v>
       </c>
@@ -55399,7 +55411,7 @@
         <f>SUM(P5:P40)</f>
         <v>3684795.48</v>
       </c>
-      <c r="Q49" s="663">
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
         <v>7.9800000000104774</v>
       </c>
@@ -55432,10 +55444,10 @@
       <c r="L50" s="378">
         <v>10278.9</v>
       </c>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>353172.5</v>
@@ -55526,11 +55538,11 @@
       <c r="L53" s="376">
         <v>28000</v>
       </c>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
         <v>2941543.98</v>
       </c>
-      <c r="N53" s="666"/>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -56009,26 +56021,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="659" t="s">
+      <c r="H77" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="660"/>
+      <c r="I77" s="673"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="661">
+      <c r="K77" s="674">
         <f>I75+L75</f>
         <v>646140.08000000031</v>
       </c>
-      <c r="L77" s="662"/>
+      <c r="L77" s="675"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="653" t="s">
+      <c r="D78" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="653"/>
+      <c r="E78" s="666"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1113109.92</v>
@@ -56037,22 +56049,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="654" t="s">
+      <c r="D79" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="654"/>
+      <c r="E79" s="667"/>
       <c r="F79" s="101">
         <v>-1405309.97</v>
       </c>
-      <c r="I79" s="655" t="s">
+      <c r="I79" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="656"/>
-      <c r="K79" s="657">
+      <c r="J79" s="669"/>
+      <c r="K79" s="670">
         <f>F81+F82+F83</f>
         <v>3400888.74</v>
       </c>
-      <c r="L79" s="657"/>
+      <c r="L79" s="670"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -56093,11 +56105,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="658">
+      <c r="K81" s="671">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="657"/>
+      <c r="L81" s="670"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -56114,22 +56126,22 @@
       <c r="C83" s="172">
         <v>45014</v>
       </c>
-      <c r="D83" s="646" t="s">
+      <c r="D83" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="647"/>
+      <c r="E83" s="660"/>
       <c r="F83" s="173">
         <v>3567993.62</v>
       </c>
-      <c r="I83" s="648" t="s">
+      <c r="I83" s="661" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="649"/>
-      <c r="K83" s="650">
+      <c r="J83" s="662"/>
+      <c r="K83" s="663">
         <f>K79+K81</f>
         <v>-103289.32999999961</v>
       </c>
-      <c r="L83" s="650"/>
+      <c r="L83" s="663"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -56276,12 +56288,6 @@
     <sortCondition ref="J46:J60"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -56298,6 +56304,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -57600,10 +57612,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I36" s="676"/>
-      <c r="J36" s="677"/>
-      <c r="K36" s="677"/>
-      <c r="L36" s="678"/>
+      <c r="I36" s="678"/>
+      <c r="J36" s="679"/>
+      <c r="K36" s="679"/>
+      <c r="L36" s="680"/>
       <c r="M36" s="101"/>
       <c r="N36" s="227">
         <f t="shared" si="1"/>
@@ -57620,10 +57632,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I37" s="676"/>
-      <c r="J37" s="677"/>
-      <c r="K37" s="677"/>
-      <c r="L37" s="678"/>
+      <c r="I37" s="678"/>
+      <c r="J37" s="679"/>
+      <c r="K37" s="679"/>
+      <c r="L37" s="680"/>
       <c r="M37" s="101"/>
       <c r="N37" s="227">
         <f t="shared" si="1"/>
@@ -57680,10 +57692,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I40" s="679" t="s">
+      <c r="I40" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="680"/>
+      <c r="J40" s="682"/>
       <c r="K40" s="84"/>
       <c r="L40" s="238"/>
       <c r="M40" s="84"/>
@@ -57702,8 +57714,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I41" s="681"/>
-      <c r="J41" s="682"/>
+      <c r="I41" s="683"/>
+      <c r="J41" s="684"/>
       <c r="K41" s="84"/>
       <c r="L41" s="238"/>
       <c r="M41" s="84"/>
@@ -57722,8 +57734,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I42" s="683"/>
-      <c r="J42" s="684"/>
+      <c r="I42" s="685"/>
+      <c r="J42" s="686"/>
       <c r="K42" s="84"/>
       <c r="L42" s="238"/>
       <c r="M42" s="84"/>
@@ -58227,10 +58239,10 @@
         <f>SUM(G3:G66)</f>
         <v>0</v>
       </c>
-      <c r="I67" s="685" t="s">
+      <c r="I67" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="686"/>
+      <c r="J67" s="688"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>103441.83</v>
@@ -58250,11 +58262,11 @@
       <c r="D68" s="268"/>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="689" t="s">
+      <c r="G68" s="691" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="694"/>
-      <c r="J68" s="695"/>
+      <c r="I68" s="696"/>
+      <c r="J68" s="697"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -58265,7 +58277,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="690"/>
+      <c r="G69" s="692"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -58871,23 +58883,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>368</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -58897,24 +58909,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="696" t="s">
+      <c r="R3" s="698" t="s">
         <v>3</v>
       </c>
     </row>
@@ -58929,14 +58941,14 @@
       <c r="D4" s="24">
         <v>45014</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -58946,11 +58958,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="697"/>
+      <c r="R4" s="699"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -60971,11 +60983,11 @@
       <c r="L49" s="49">
         <v>25617.51</v>
       </c>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
         <v>2051765.3</v>
       </c>
-      <c r="N49" s="651">
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
         <v>1741324</v>
       </c>
@@ -60983,7 +60995,7 @@
         <f>SUM(P5:P40)</f>
         <v>4831473.13</v>
       </c>
-      <c r="Q49" s="663">
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
         <v>-111.39999999999418</v>
       </c>
@@ -61010,10 +61022,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>97872.53</v>
@@ -61087,11 +61099,11 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
         <v>3793089.3</v>
       </c>
-      <c r="N53" s="666"/>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -61720,26 +61732,26 @@
       <c r="A79" s="152"/>
       <c r="B79" s="153"/>
       <c r="C79" s="1"/>
-      <c r="H79" s="659" t="s">
+      <c r="H79" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I79" s="660"/>
+      <c r="I79" s="673"/>
       <c r="J79" s="154"/>
-      <c r="K79" s="661">
+      <c r="K79" s="674">
         <f>I77+L77</f>
         <v>739761.38</v>
       </c>
-      <c r="L79" s="662"/>
+      <c r="L79" s="675"/>
       <c r="M79" s="155"/>
       <c r="N79" s="155"/>
       <c r="P79" s="44"/>
       <c r="Q79" s="19"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D80" s="653" t="s">
+      <c r="D80" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E80" s="653"/>
+      <c r="E80" s="666"/>
       <c r="F80" s="156">
         <f>F77-K79-C77</f>
         <v>2011425.4899999998</v>
@@ -61748,22 +61760,22 @@
       <c r="J80" s="158"/>
     </row>
     <row r="81" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D81" s="654" t="s">
+      <c r="D81" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="654"/>
+      <c r="E81" s="667"/>
       <c r="F81" s="101">
         <v>-2021696.34</v>
       </c>
-      <c r="I81" s="655" t="s">
+      <c r="I81" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J81" s="656"/>
-      <c r="K81" s="657">
+      <c r="J81" s="669"/>
+      <c r="K81" s="670">
         <f>F83+F84+F85</f>
         <v>2945239.9399999995</v>
       </c>
-      <c r="L81" s="657"/>
+      <c r="L81" s="670"/>
       <c r="M81" s="159"/>
       <c r="N81" s="159"/>
       <c r="O81" s="160"/>
@@ -61804,11 +61816,11 @@
         <v>21</v>
       </c>
       <c r="J83" s="170"/>
-      <c r="K83" s="658">
+      <c r="K83" s="671">
         <f>-C4</f>
         <v>-3567993.62</v>
       </c>
-      <c r="L83" s="657"/>
+      <c r="L83" s="670"/>
     </row>
     <row r="84" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="171" t="s">
@@ -61825,22 +61837,22 @@
       <c r="C85" s="172">
         <v>45051</v>
       </c>
-      <c r="D85" s="646" t="s">
+      <c r="D85" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E85" s="647"/>
+      <c r="E85" s="660"/>
       <c r="F85" s="173">
         <v>3065283.79</v>
       </c>
-      <c r="I85" s="648" t="s">
+      <c r="I85" s="661" t="s">
         <v>220</v>
       </c>
-      <c r="J85" s="649"/>
-      <c r="K85" s="650">
+      <c r="J85" s="662"/>
+      <c r="K85" s="663">
         <f>K81+K83</f>
         <v>-622753.68000000063</v>
       </c>
-      <c r="L85" s="650"/>
+      <c r="L85" s="663"/>
     </row>
     <row r="86" spans="2:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C86" s="174"/>
@@ -61988,6 +62000,12 @@
     <sortCondition ref="B45:B61"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -62004,12 +62022,6 @@
     <mergeCell ref="H79:I79"/>
     <mergeCell ref="K79:L79"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -63329,10 +63341,10 @@
         <f t="shared" si="0"/>
         <v>10327.200000000001</v>
       </c>
-      <c r="I36" s="676"/>
-      <c r="J36" s="677"/>
-      <c r="K36" s="677"/>
-      <c r="L36" s="678"/>
+      <c r="I36" s="678"/>
+      <c r="J36" s="679"/>
+      <c r="K36" s="679"/>
+      <c r="L36" s="680"/>
       <c r="M36" s="101"/>
       <c r="N36" s="227">
         <f t="shared" si="1"/>
@@ -63355,10 +63367,10 @@
         <f t="shared" si="0"/>
         <v>63383.41</v>
       </c>
-      <c r="I37" s="676"/>
-      <c r="J37" s="677"/>
-      <c r="K37" s="677"/>
-      <c r="L37" s="678"/>
+      <c r="I37" s="678"/>
+      <c r="J37" s="679"/>
+      <c r="K37" s="679"/>
+      <c r="L37" s="680"/>
       <c r="M37" s="101"/>
       <c r="N37" s="227">
         <f t="shared" si="1"/>
@@ -63433,10 +63445,10 @@
         <f t="shared" si="0"/>
         <v>10162.64</v>
       </c>
-      <c r="I40" s="679" t="s">
+      <c r="I40" s="681" t="s">
         <v>35</v>
       </c>
-      <c r="J40" s="680"/>
+      <c r="J40" s="682"/>
       <c r="K40" s="84"/>
       <c r="L40" s="238"/>
       <c r="M40" s="84"/>
@@ -63461,8 +63473,8 @@
         <f t="shared" si="0"/>
         <v>12934.8</v>
       </c>
-      <c r="I41" s="681"/>
-      <c r="J41" s="682"/>
+      <c r="I41" s="683"/>
+      <c r="J41" s="684"/>
       <c r="K41" s="84"/>
       <c r="L41" s="238"/>
       <c r="M41" s="84"/>
@@ -63487,8 +63499,8 @@
         <f t="shared" si="0"/>
         <v>35275.5</v>
       </c>
-      <c r="I42" s="683"/>
-      <c r="J42" s="684"/>
+      <c r="I42" s="685"/>
+      <c r="J42" s="686"/>
       <c r="K42" s="84"/>
       <c r="L42" s="238"/>
       <c r="M42" s="84"/>
@@ -64010,10 +64022,10 @@
         <f>SUM(G3:G66)</f>
         <v>1592169.2799999998</v>
       </c>
-      <c r="I67" s="685" t="s">
+      <c r="I67" s="687" t="s">
         <v>35</v>
       </c>
-      <c r="J67" s="686"/>
+      <c r="J67" s="688"/>
       <c r="K67" s="264">
         <f>SUM(K3:K66)</f>
         <v>121598</v>
@@ -64033,11 +64045,11 @@
       <c r="D68" s="268"/>
       <c r="E68" s="269"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="689" t="s">
+      <c r="G68" s="691" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="694"/>
-      <c r="J68" s="695"/>
+      <c r="I68" s="696"/>
+      <c r="J68" s="697"/>
       <c r="K68" s="1"/>
       <c r="L68" s="269"/>
       <c r="M68" s="5"/>
@@ -64048,7 +64060,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="269"/>
       <c r="F69" s="5"/>
-      <c r="G69" s="690"/>
+      <c r="G69" s="692"/>
       <c r="I69" s="293"/>
       <c r="J69" s="294"/>
       <c r="K69" s="295"/>
@@ -64664,23 +64676,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="669"/>
-      <c r="C1" s="671" t="s">
+      <c r="B1" s="646"/>
+      <c r="C1" s="648" t="s">
         <v>502</v>
       </c>
-      <c r="D1" s="672"/>
-      <c r="E1" s="672"/>
-      <c r="F1" s="672"/>
-      <c r="G1" s="672"/>
-      <c r="H1" s="672"/>
-      <c r="I1" s="672"/>
-      <c r="J1" s="672"/>
-      <c r="K1" s="672"/>
-      <c r="L1" s="672"/>
-      <c r="M1" s="672"/>
+      <c r="D1" s="649"/>
+      <c r="E1" s="649"/>
+      <c r="F1" s="649"/>
+      <c r="G1" s="649"/>
+      <c r="H1" s="649"/>
+      <c r="I1" s="649"/>
+      <c r="J1" s="649"/>
+      <c r="K1" s="649"/>
+      <c r="L1" s="649"/>
+      <c r="M1" s="649"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="670"/>
+      <c r="B2" s="647"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -64690,27 +64702,27 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="673" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="674"/>
+      <c r="B3" s="650" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="651"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="675" t="s">
+      <c r="H3" s="652" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="675"/>
+      <c r="I3" s="652"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="667" t="s">
+      <c r="P3" s="644" t="s">
         <v>2</v>
       </c>
       <c r="Q3" s="467" t="s">
         <v>509</v>
       </c>
-      <c r="R3" s="696" t="s">
+      <c r="R3" s="698" t="s">
         <v>3</v>
       </c>
     </row>
@@ -64725,14 +64737,14 @@
       <c r="D4" s="24">
         <v>45051</v>
       </c>
-      <c r="E4" s="642" t="s">
+      <c r="E4" s="655" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="643"/>
-      <c r="H4" s="644" t="s">
+      <c r="F4" s="656"/>
+      <c r="H4" s="657" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="645"/>
+      <c r="I4" s="658"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -64742,11 +64754,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="668"/>
+      <c r="P4" s="645"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="697"/>
+      <c r="R4" s="699"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -66749,11 +66761,11 @@
       <c r="L49" s="49">
         <v>8091</v>
       </c>
-      <c r="M49" s="651">
+      <c r="M49" s="664">
         <f>SUM(M5:M40)</f>
         <v>1683911.56</v>
       </c>
-      <c r="N49" s="651">
+      <c r="N49" s="664">
         <f>SUM(N5:N40)</f>
         <v>1355406.15</v>
       </c>
@@ -66761,7 +66773,7 @@
         <f>SUM(P5:P40)</f>
         <v>3685318.7</v>
       </c>
-      <c r="Q49" s="663">
+      <c r="Q49" s="676">
         <f>SUM(Q5:Q40)</f>
         <v>5790.6999999999971</v>
       </c>
@@ -66794,10 +66806,10 @@
       <c r="L50" s="89">
         <v>1856</v>
       </c>
-      <c r="M50" s="652"/>
-      <c r="N50" s="652"/>
+      <c r="M50" s="665"/>
+      <c r="N50" s="665"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="664"/>
+      <c r="Q50" s="677"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>13930</v>
@@ -66876,11 +66888,11 @@
       <c r="L53" s="49">
         <v>9804.18</v>
       </c>
-      <c r="M53" s="665">
+      <c r="M53" s="642">
         <f>M49+N49</f>
         <v>3039317.71</v>
       </c>
-      <c r="N53" s="666"/>
+      <c r="N53" s="643"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -67359,26 +67371,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="659" t="s">
+      <c r="H77" s="672" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="660"/>
+      <c r="I77" s="673"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="661">
+      <c r="K77" s="674">
         <f>I75+L75</f>
         <v>484126.00999999989</v>
       </c>
-      <c r="L77" s="662"/>
+      <c r="L77" s="675"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="653" t="s">
+      <c r="D78" s="666" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="653"/>
+      <c r="E78" s="666"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1743477.6000000003</v>
@@ -67387,22 +67399,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="654" t="s">
+      <c r="D79" s="667" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="654"/>
+      <c r="E79" s="667"/>
       <c r="F79" s="101">
         <v>-1542483.8</v>
       </c>
-      <c r="I79" s="655" t="s">
+      <c r="I79" s="668" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="656"/>
-      <c r="K79" s="657">
+      <c r="J79" s="669"/>
+      <c r="K79" s="670">
         <f>F81+F82+F83</f>
         <v>4235033.33</v>
       </c>
-      <c r="L79" s="657"/>
+      <c r="L79" s="670"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -67443,11 +67455,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="658">
+      <c r="K81" s="671">
         <f>-C4</f>
         <v>-3065283.79</v>
       </c>
-      <c r="L81" s="657"/>
+      <c r="L81" s="670"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -67464,22 +67476,22 @@
       <c r="C83" s="172">
         <v>45079</v>
       </c>
-      <c r="D83" s="646" t="s">
+      <c r="D83" s="659" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="647"/>
+      <c r="E83" s="660"/>
       <c r="F83" s="173">
         <v>3897967.53</v>
       </c>
-      <c r="I83" s="691" t="s">
+      <c r="I83" s="693" t="s">
         <v>25</v>
       </c>
-      <c r="J83" s="692"/>
-      <c r="K83" s="693">
+      <c r="J83" s="694"/>
+      <c r="K83" s="695">
         <f>K79+K81</f>
         <v>1169749.54</v>
       </c>
-      <c r="L83" s="693"/>
+      <c r="L83" s="695"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -67627,12 +67639,6 @@
     <sortCondition ref="J46:J62"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -67649,6 +67655,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.31496062992125984" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="85" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>